<commit_message>
updated fern physiology for data table
</commit_message>
<xml_diff>
--- a/extras/extra_fern.xlsx
+++ b/extras/extra_fern.xlsx
@@ -601,7 +601,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -613,6 +613,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -636,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -644,6 +651,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -924,15 +932,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -955,7 +963,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -977,8 +985,24 @@
       <c r="G2">
         <v>500</v>
       </c>
+      <c r="I2">
+        <f>AVERAGE(C2:C6)</f>
+        <v>3.3081940384578195</v>
+      </c>
+      <c r="J2">
+        <f>AVERAGE(D2:D6)</f>
+        <v>6.7446743883419494E-2</v>
+      </c>
+      <c r="K2">
+        <f>(STDEV(C2:C6))/(SQRT(COUNT(C2:C6)))</f>
+        <v>0.35279426275521902</v>
+      </c>
+      <c r="L2">
+        <f>(STDEV(D2:D6))/(SQRT(COUNT(D2:D6)))</f>
+        <v>1.687484111112892E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1001,7 +1025,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1024,7 +1048,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1047,7 +1071,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1070,7 +1094,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1092,8 +1116,24 @@
       <c r="G8">
         <v>500</v>
       </c>
+      <c r="I8">
+        <f>AVERAGE(C8:C12)</f>
+        <v>3.2181715686320169</v>
+      </c>
+      <c r="J8">
+        <f>AVERAGE(D8:D12)</f>
+        <v>6.2812795773844937E-2</v>
+      </c>
+      <c r="K8" s="3">
+        <f>(STDEV(C8:C12))/(SQRT(COUNT(C8:C12)))</f>
+        <v>0.22421898821870234</v>
+      </c>
+      <c r="L8" s="3">
+        <f>(STDEV(D8:D12))/(SQRT(COUNT(D8:D12)))</f>
+        <v>6.8698311619643498E-3</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1116,7 +1156,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1139,7 +1179,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1162,7 +1202,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1187,6 +1227,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>